<commit_message>
added a feature that support persian title on import excel the
</commit_message>
<xml_diff>
--- a/TestProject1/ColumnWithBoolNotNull.xlsx
+++ b/TestProject1/ColumnWithBoolNotNull.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CMI\BackEnd\TestProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8A1449-CDE0-4DA0-BC50-B2EFC1C8DBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C1FFEA-3FFA-4D68-891E-641D2BAE17AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4845" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,19 +27,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
     <t>غیر فعال</t>
   </si>
   <si>
     <t>فعال</t>
+  </si>
+  <si>
+    <t>ستون اول</t>
+  </si>
+  <si>
+    <t>ستون دوم</t>
+  </si>
+  <si>
+    <t>ستون سوم</t>
   </si>
 </sst>
 </file>
@@ -360,20 +360,20 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -381,7 +381,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -406,7 +406,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>